<commit_message>
Site updated: 2020-04-17 15:40:02
</commit_message>
<xml_diff>
--- a/文档备注.xlsx
+++ b/文档备注.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136">
   <si>
     <t>文件名</t>
   </si>
@@ -368,6 +368,60 @@
   </si>
   <si>
     <t>2020 蓝桥杯大学模拟赛(二) - 程序设计：植物大战僵尸</t>
+  </si>
+  <si>
+    <t>qipanfugaiwenti</t>
+  </si>
+  <si>
+    <t>棋盘覆盖问题——算法设计课程</t>
+  </si>
+  <si>
+    <t>big-int-multiply</t>
+  </si>
+  <si>
+    <t>大整数乘法思想——算法设计课程</t>
+  </si>
+  <si>
+    <t>lanqiaobei3-fenpisa</t>
+  </si>
+  <si>
+    <t>2020 蓝桥杯大学模拟赛(三) - 程序设计：分披萨</t>
+  </si>
+  <si>
+    <t>lanqiaobei3-yangmao</t>
+  </si>
+  <si>
+    <t>2020 蓝桥杯大学模拟赛(三) - 程序设计：养猫</t>
+  </si>
+  <si>
+    <t>lanqiaobei3-tupozhangai</t>
+  </si>
+  <si>
+    <t>2020 蓝桥杯大学模拟赛(三) - 程序设计：突破障碍</t>
+  </si>
+  <si>
+    <t>buy-aliyun-process</t>
+  </si>
+  <si>
+    <t>购买阿里云服务器流程</t>
+  </si>
+  <si>
+    <t>configure-blog-to-aliyunserver</t>
+  </si>
+  <si>
+    <t>hexo个人博客搭建到阿里云服务器</t>
+  </si>
+  <si>
+    <t>LCS-continuously</t>
+  </si>
+  <si>
+    <t>LCS——最长公共子序列“连续”与“不连续”版本</t>
+  </si>
+  <si>
+    <t>Integer-Factorization</t>
+  </si>
+  <si>
+    <t>整数因子分解——算法设计课程</t>
   </si>
 </sst>
 </file>
@@ -376,9 +430,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -403,21 +457,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -431,6 +471,75 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -439,30 +548,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -479,6 +564,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -488,63 +587,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -561,37 +615,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -603,49 +735,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -657,7 +753,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,73 +771,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,26 +806,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -791,17 +842,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -822,27 +878,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -851,152 +905,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1005,9 +1059,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1340,10 +1391,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="1"/>
@@ -1362,162 +1413,162 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1525,7 +1576,7 @@
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1533,7 +1584,7 @@
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1541,7 +1592,7 @@
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1549,7 +1600,7 @@
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1557,7 +1608,7 @@
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1565,7 +1616,7 @@
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1573,7 +1624,7 @@
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1581,7 +1632,7 @@
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1589,7 +1640,7 @@
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1597,7 +1648,7 @@
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1605,7 +1656,7 @@
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1613,7 +1664,7 @@
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1621,7 +1672,7 @@
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1629,7 +1680,7 @@
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1637,7 +1688,7 @@
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1645,7 +1696,7 @@
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1653,7 +1704,7 @@
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1661,7 +1712,7 @@
       <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1669,7 +1720,7 @@
       <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1677,7 +1728,7 @@
       <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1685,7 +1736,7 @@
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1693,7 +1744,7 @@
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1701,7 +1752,7 @@
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1709,7 +1760,7 @@
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1717,7 +1768,7 @@
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1725,7 +1776,7 @@
       <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1733,7 +1784,7 @@
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1741,7 +1792,7 @@
       <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="4" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1749,7 +1800,7 @@
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1757,7 +1808,7 @@
       <c r="A51" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1765,7 +1816,7 @@
       <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1773,7 +1824,7 @@
       <c r="A53" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="4" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1781,7 +1832,7 @@
       <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1789,7 +1840,7 @@
       <c r="A55" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="4" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1797,7 +1848,7 @@
       <c r="A56" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="5" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1805,7 +1856,7 @@
       <c r="A57" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="4" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1813,7 +1864,7 @@
       <c r="A58" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="6" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1821,8 +1872,80 @@
       <c r="A59" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="6" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2020-04-17 16:34:03
</commit_message>
<xml_diff>
--- a/文档备注.xlsx
+++ b/文档备注.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138">
   <si>
     <t>文件名</t>
   </si>
@@ -422,6 +422,12 @@
   </si>
   <si>
     <t>整数因子分解——算法设计课程</t>
+  </si>
+  <si>
+    <t>UML-UseCase</t>
+  </si>
+  <si>
+    <t>UML学习笔记——用例图</t>
   </si>
 </sst>
 </file>
@@ -1391,10 +1397,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="1"/>
@@ -1948,6 +1954,14 @@
         <v>135</v>
       </c>
     </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2020-04-21 08:32:20
</commit_message>
<xml_diff>
--- a/文档备注.xlsx
+++ b/文档备注.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12100"/>
+    <workbookView windowWidth="24720" windowHeight="11200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140">
   <si>
     <t>文件名</t>
   </si>
@@ -428,6 +428,12 @@
   </si>
   <si>
     <t>UML学习笔记——用例图</t>
+  </si>
+  <si>
+    <t>UML-ClassDiagram</t>
+  </si>
+  <si>
+    <t>UML学习笔记——类图</t>
   </si>
 </sst>
 </file>
@@ -435,10 +441,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -463,7 +469,59 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -477,6 +535,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -485,8 +589,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -500,111 +605,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -621,25 +627,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,61 +777,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,79 +801,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -812,8 +818,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -829,6 +850,41 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -850,59 +906,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -911,34 +917,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -947,112 +956,109 @@
     <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1397,7 +1403,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
       <selection activeCell="B70" sqref="B70"/>
@@ -1962,6 +1968,14 @@
         <v>137</v>
       </c>
     </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2020-04-23 09:30:49
</commit_message>
<xml_diff>
--- a/文档备注.xlsx
+++ b/文档备注.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24720" windowHeight="11200"/>
+    <workbookView windowWidth="24780" windowHeight="11200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -441,10 +441,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -476,6 +476,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -490,20 +512,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -512,6 +520,90 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -519,98 +611,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -621,187 +621,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -824,17 +824,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -850,30 +844,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -904,11 +874,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -917,145 +917,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1405,8 +1405,8 @@
   <sheetPr/>
   <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
Site updated: 2020-04-24 08:35:25
</commit_message>
<xml_diff>
--- a/文档备注.xlsx
+++ b/文档备注.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24780" windowHeight="11200"/>
+    <workbookView windowWidth="25600" windowHeight="12100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142">
   <si>
     <t>文件名</t>
   </si>
@@ -434,6 +434,12 @@
   </si>
   <si>
     <t>UML学习笔记——类图</t>
+  </si>
+  <si>
+    <t>Matrix-Multiplication</t>
+  </si>
+  <si>
+    <t>矩阵连乘问题——算法设计课程</t>
   </si>
 </sst>
 </file>
@@ -443,8 +449,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -469,21 +475,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -497,8 +489,122 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -511,106 +617,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -621,187 +627,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -818,8 +824,38 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -828,22 +864,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -874,40 +895,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -917,148 +923,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1403,10 +1409,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="1"/>
@@ -1976,6 +1982,14 @@
         <v>139</v>
       </c>
     </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Site updated: 2020-04-24 15:29:01
</commit_message>
<xml_diff>
--- a/文档备注.xlsx
+++ b/文档备注.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12100"/>
+    <workbookView windowWidth="25600" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146">
   <si>
     <t>文件名</t>
   </si>
@@ -440,6 +440,18 @@
   </si>
   <si>
     <t>矩阵连乘问题——算法设计课程</t>
+  </si>
+  <si>
+    <t>UML-SequenceDiagram</t>
+  </si>
+  <si>
+    <t>UML学习笔记——顺序图（时序图）</t>
+  </si>
+  <si>
+    <t>find-similar-string</t>
+  </si>
+  <si>
+    <t>找相似串问题——算法设计课程</t>
   </si>
 </sst>
 </file>
@@ -447,9 +459,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -475,7 +487,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -489,6 +515,91 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -504,85 +615,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -593,30 +629,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -633,181 +645,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -824,38 +836,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -864,18 +846,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -898,8 +869,49 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -923,148 +935,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1409,10 +1421,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="1"/>
@@ -1990,6 +2002,22 @@
         <v>141</v>
       </c>
     </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>